<commit_message>
Add missing decryption runtime and clean up runtime separators
</commit_message>
<xml_diff>
--- a/docs/Analyses.xlsx
+++ b/docs/Analyses.xlsx
@@ -463,7 +463,7 @@
         <v>-17854.32704906508</v>
       </c>
       <c r="C2" t="n">
-        <v>-17854.32704906372</v>
+        <v>-17854.32704906524</v>
       </c>
     </row>
     <row r="3">
@@ -476,7 +476,7 @@
         <v>14042.59545713267</v>
       </c>
       <c r="C3" t="n">
-        <v>14042.59545713286</v>
+        <v>14042.59545713462</v>
       </c>
     </row>
     <row r="4">
@@ -489,7 +489,7 @@
         <v>5513.877038820377</v>
       </c>
       <c r="C4" t="n">
-        <v>5513.877038819353</v>
+        <v>5513.877038814026</v>
       </c>
     </row>
     <row r="5">
@@ -502,7 +502,7 @@
         <v>4701.11754893352</v>
       </c>
       <c r="C5" t="n">
-        <v>4701.117548933131</v>
+        <v>4701.117548934597</v>
       </c>
     </row>
     <row r="6">
@@ -515,7 +515,7 @@
         <v>4363.940245938234</v>
       </c>
       <c r="C6" t="n">
-        <v>4363.940245938426</v>
+        <v>4363.940245938534</v>
       </c>
     </row>
     <row r="7">
@@ -528,7 +528,7 @@
         <v>-4350.725522799707</v>
       </c>
       <c r="C7" t="n">
-        <v>-4350.725522799443</v>
+        <v>-4350.72552279905</v>
       </c>
     </row>
     <row r="8">
@@ -541,7 +541,7 @@
         <v>-2201.599338927801</v>
       </c>
       <c r="C8" t="n">
-        <v>-2201.59933892755</v>
+        <v>-2201.599338929234</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>-1364.822336428711</v>
       </c>
       <c r="C9" t="n">
-        <v>-1364.822336427345</v>
+        <v>-1364.822336431141</v>
       </c>
     </row>
     <row r="10">
@@ -567,7 +567,7 @@
         <v>-427.6614785965969</v>
       </c>
       <c r="C10" t="n">
-        <v>-427.6614785933641</v>
+        <v>-427.661478598414</v>
       </c>
     </row>
     <row r="11">
@@ -580,7 +580,7 @@
         <v>-321.2333687690991</v>
       </c>
       <c r="C11" t="n">
-        <v>-321.2333687682541</v>
+        <v>-321.2333687677409</v>
       </c>
     </row>
     <row r="12">
@@ -593,7 +593,7 @@
         <v>-201.7694550903941</v>
       </c>
       <c r="C12" t="n">
-        <v>-201.7694550917827</v>
+        <v>-201.7694550906396</v>
       </c>
     </row>
     <row r="13">
@@ -606,7 +606,7 @@
         <v>201.2629543634045</v>
       </c>
       <c r="C13" t="n">
-        <v>201.2629543639775</v>
+        <v>201.2629543625523</v>
       </c>
     </row>
     <row r="14">
@@ -619,7 +619,7 @@
         <v>185.0718710649574</v>
       </c>
       <c r="C14" t="n">
-        <v>185.0718710665301</v>
+        <v>185.0718710626106</v>
       </c>
     </row>
     <row r="15">
@@ -632,7 +632,7 @@
         <v>151.5601082708775</v>
       </c>
       <c r="C15" t="n">
-        <v>151.5601082704297</v>
+        <v>151.5601082696767</v>
       </c>
     </row>
     <row r="16">
@@ -645,7 +645,7 @@
         <v>143.0183857681953</v>
       </c>
       <c r="C16" t="n">
-        <v>143.0183857681083</v>
+        <v>143.0183857675093</v>
       </c>
     </row>
     <row r="17">
@@ -658,7 +658,7 @@
         <v>114.7607661655936</v>
       </c>
       <c r="C17" t="n">
-        <v>114.7607661656252</v>
+        <v>114.7607661645206</v>
       </c>
     </row>
     <row r="18">
@@ -671,7 +671,7 @@
         <v>10.5973762821793</v>
       </c>
       <c r="C18" t="n">
-        <v>10.59737627951472</v>
+        <v>10.59737628136645</v>
       </c>
     </row>
     <row r="19">
@@ -684,7 +684,7 @@
         <v>-7.089485867176286</v>
       </c>
       <c r="C19" t="n">
-        <v>-7.089485867392796</v>
+        <v>-7.089485865492861</v>
       </c>
     </row>
     <row r="20">
@@ -697,7 +697,7 @@
         <v>6.209684235855929</v>
       </c>
       <c r="C20" t="n">
-        <v>6.209684234856923</v>
+        <v>6.209684236669091</v>
       </c>
     </row>
     <row r="21">
@@ -710,7 +710,7 @@
         <v>-0.2926168164095956</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.2926168170524761</v>
+        <v>-0.2926168162575777</v>
       </c>
     </row>
     <row r="22">
@@ -723,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>1.934976623374496e-10</v>
+        <v>-1.064549337570497e-09</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +772,7 @@
         <v>2.473499997637179</v>
       </c>
       <c r="C2" t="n">
-        <v>2.4735011171548</v>
+        <v>2.473501344543386</v>
       </c>
     </row>
     <row r="3">
@@ -785,7 +785,7 @@
         <v>15.02766651526452</v>
       </c>
       <c r="C3" t="n">
-        <v>15.0277092978497</v>
+        <v>15.0277061464848</v>
       </c>
     </row>
     <row r="4">
@@ -798,7 +798,7 @@
         <v>3.876553432530567</v>
       </c>
       <c r="C4" t="n">
-        <v>3.876558950648074</v>
+        <v>3.876558544183848</v>
       </c>
     </row>
     <row r="5">
@@ -811,7 +811,7 @@
         <v>0.9263893126590724</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9263891030952324</v>
+        <v>0.9263891185317032</v>
       </c>
     </row>
   </sheetData>
@@ -825,7 +825,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>0.4194540977478027</v>
+        <v>0.4714062213897705</v>
       </c>
     </row>
     <row r="3">
@@ -868,10 +868,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.599197149276733</v>
+        <v>3.666933059692383</v>
       </c>
       <c r="C3" t="n">
-        <v>4.24517822265625</v>
+        <v>5.661703824996948</v>
       </c>
     </row>
     <row r="4">
@@ -881,49 +881,71 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.00195002555847168</v>
+        <v>0.004482507705688477</v>
       </c>
       <c r="C4" t="n">
-        <v>0.00195002555847168</v>
+        <v>0.004482507705688477</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Evaluation Time</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
+          <t>Encryption Time</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
-        <v>13.35389757156372</v>
+        <v>4.491698265075684</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Total without preprocessing</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.00195002555847168</v>
-      </c>
+          <t>Decryption Time</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>18.01852989196777</v>
+        <v>0.6985993385314941</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Evaluation Time</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>14.0158166885376</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Total without initial preprocessing</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.004482507705688477</v>
+      </c>
+      <c r="C8" t="n">
+        <v>19.67752051353455</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>Total Runtime</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>3.601147174835205</v>
-      </c>
-      <c r="C7" t="n">
-        <v>21.61967706680298</v>
+      <c r="B9" t="n">
+        <v>3.671415567398071</v>
+      </c>
+      <c r="C9" t="n">
+        <v>23.34893608093262</v>
       </c>
     </row>
   </sheetData>
@@ -972,7 +994,7 @@
         <v>0.1640625</v>
       </c>
       <c r="C2" t="n">
-        <v>326.38671875</v>
+        <v>326.1572265625</v>
       </c>
     </row>
     <row r="3">
@@ -985,7 +1007,7 @@
         <v>0.03125</v>
       </c>
       <c r="C3" t="n">
-        <v>229.8759765625</v>
+        <v>229.923828125</v>
       </c>
     </row>
     <row r="4">
@@ -998,7 +1020,7 @@
         <v>129.9375</v>
       </c>
       <c r="C4" t="n">
-        <v>258581.6845703125</v>
+        <v>258581.541015625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>